<commit_message>
changed the chart of the second day's score
</commit_message>
<xml_diff>
--- a/Docs/计分组/day2计分表.xlsx
+++ b/Docs/计分组/day2计分表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\栩海\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git work\2015-Tsinghua-XLP-CDT\Docs\计分组\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>郝育昆</t>
   </si>
@@ -236,12 +236,81 @@
     <t>备注</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>day1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>总分</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>组员互相平分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第一次</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记分组评分
+第一次</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +338,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -305,7 +381,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -331,6 +407,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -613,531 +695,646 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9" style="7"/>
-    <col min="6" max="6" width="15.625" style="7" customWidth="1"/>
-    <col min="7" max="10" width="9" style="7"/>
-    <col min="11" max="11" width="15.875" style="7" customWidth="1"/>
-    <col min="12" max="13" width="13" style="7" customWidth="1"/>
-    <col min="14" max="14" width="16.5" style="7" customWidth="1"/>
-    <col min="15" max="15" width="11.125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="9" style="7"/>
-    <col min="17" max="17" width="19.375" style="7" customWidth="1"/>
-    <col min="18" max="19" width="9" style="7"/>
-    <col min="20" max="20" width="16.875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="13.875" style="7" customWidth="1"/>
-    <col min="22" max="22" width="9" style="7"/>
-    <col min="23" max="23" width="17.5" style="7" customWidth="1"/>
-    <col min="24" max="26" width="9" style="7"/>
-    <col min="27" max="27" width="18.125" style="7" customWidth="1"/>
-    <col min="28" max="16384" width="9" style="7"/>
+    <col min="2" max="4" width="17.75" style="10" customWidth="1"/>
+    <col min="5" max="8" width="9" style="7"/>
+    <col min="9" max="9" width="15.625" style="7" customWidth="1"/>
+    <col min="10" max="13" width="9" style="7"/>
+    <col min="14" max="14" width="15.875" style="7" customWidth="1"/>
+    <col min="15" max="16" width="13" style="7" customWidth="1"/>
+    <col min="17" max="17" width="16.5" style="7" customWidth="1"/>
+    <col min="18" max="18" width="11.125" style="7" customWidth="1"/>
+    <col min="19" max="19" width="9" style="7"/>
+    <col min="20" max="20" width="19.375" style="7" customWidth="1"/>
+    <col min="21" max="22" width="9" style="7"/>
+    <col min="23" max="23" width="16.875" style="7" customWidth="1"/>
+    <col min="24" max="24" width="13.875" style="7" customWidth="1"/>
+    <col min="25" max="25" width="9" style="7"/>
+    <col min="26" max="26" width="17.5" style="7" customWidth="1"/>
+    <col min="27" max="29" width="9" style="7"/>
+    <col min="30" max="30" width="18.125" style="7" customWidth="1"/>
+    <col min="31" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:31" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="X1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="I2" s="8"/>
       <c r="N2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="T2" s="8"/>
       <c r="W2" s="8"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z2" s="8"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="I3" s="8"/>
       <c r="N3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="T3" s="8"/>
       <c r="W3" s="8"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z3" s="8"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="I4" s="8"/>
       <c r="N4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="T4" s="8"/>
       <c r="W4" s="8"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z4" s="8"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="I5" s="8"/>
       <c r="N5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="T5" s="8"/>
       <c r="W5" s="8"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z5" s="8"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="I6" s="8"/>
       <c r="N6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="T6" s="8"/>
       <c r="W6" s="8"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z6" s="8"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="I7" s="8"/>
       <c r="N7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="T7" s="8"/>
       <c r="W7" s="8"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z7" s="8"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="I8" s="8"/>
       <c r="N8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="T8" s="8"/>
       <c r="W8" s="8"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="I9" s="8"/>
       <c r="N9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="T9" s="8"/>
       <c r="W9" s="8"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z9" s="8"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="I10" s="8"/>
       <c r="N10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="T10" s="8"/>
       <c r="W10" s="8"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z10" s="8"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="I11" s="8"/>
       <c r="N11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="T11" s="8"/>
       <c r="W11" s="8"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z11" s="8"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="I12" s="8"/>
       <c r="N12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="T12" s="8"/>
       <c r="W12" s="8"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="I13" s="8"/>
       <c r="N13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="T13" s="8"/>
       <c r="W13" s="8"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="I14" s="8"/>
       <c r="N14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="T14" s="8"/>
       <c r="W14" s="8"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="I15" s="8"/>
       <c r="N15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="T15" s="8"/>
       <c r="W15" s="8"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z15" s="8"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="I16" s="8"/>
       <c r="N16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="T16" s="8"/>
       <c r="W16" s="8"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z16" s="8"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="I17" s="8"/>
       <c r="N17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="T17" s="8"/>
       <c r="W17" s="8"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z17" s="8"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="I18" s="8"/>
       <c r="N18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="T18" s="8"/>
       <c r="W18" s="8"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="I19" s="8"/>
       <c r="N19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="T19" s="8"/>
       <c r="W19" s="8"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="I20" s="8"/>
       <c r="N20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="T20" s="8"/>
       <c r="W20" s="8"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="I21" s="8"/>
       <c r="N21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="T21" s="8"/>
       <c r="W21" s="8"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z21" s="8"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="I22" s="8"/>
       <c r="N22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="T22" s="8"/>
       <c r="W22" s="8"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z22" s="8"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="I23" s="8"/>
       <c r="N23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="T23" s="8"/>
       <c r="W23" s="8"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z23" s="8"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="I24" s="8"/>
       <c r="N24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="T24" s="8"/>
       <c r="W24" s="8"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z24" s="8"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="I25" s="8"/>
       <c r="N25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="T25" s="8"/>
       <c r="W25" s="8"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z25" s="8"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="I26" s="8"/>
       <c r="N26" s="8"/>
       <c r="Q26" s="8"/>
       <c r="T26" s="8"/>
       <c r="W26" s="8"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z26" s="8"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="I27" s="8"/>
       <c r="N27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="T27" s="8"/>
       <c r="W27" s="8"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z27" s="8"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="I28" s="8"/>
       <c r="N28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="T28" s="8"/>
       <c r="W28" s="8"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z28" s="8"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="I29" s="8"/>
       <c r="N29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="T29" s="8"/>
       <c r="W29" s="8"/>
-    </row>
-    <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.15">
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="I30" s="8"/>
       <c r="N30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="T30" s="8"/>
       <c r="W30" s="8"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="8"/>
       <c r="N31" s="8"/>
       <c r="Q31" s="8"/>
       <c r="T31" s="8"/>
       <c r="W31" s="8"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z31" s="8"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="K32" s="8"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="I32" s="8"/>
       <c r="N32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="T32" s="8"/>
       <c r="W32" s="8"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="K33" s="8"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="I33" s="8"/>
       <c r="N33" s="8"/>
       <c r="Q33" s="8"/>
       <c r="T33" s="8"/>
       <c r="W33" s="8"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="K34" s="8"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="I34" s="8"/>
       <c r="N34" s="8"/>
       <c r="Q34" s="8"/>
       <c r="T34" s="8"/>
       <c r="W34" s="8"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="I35" s="8"/>
       <c r="N35" s="8"/>
       <c r="Q35" s="8"/>
       <c r="T35" s="8"/>
       <c r="W35" s="8"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="I36" s="8"/>
       <c r="N36" s="8"/>
       <c r="Q36" s="8"/>
       <c r="T36" s="8"/>
       <c r="W36" s="8"/>
+      <c r="Z36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I2:I9"/>
+    <mergeCell ref="I10:I18"/>
+    <mergeCell ref="I19:I27"/>
+    <mergeCell ref="I28:I36"/>
+    <mergeCell ref="N2:N9"/>
+    <mergeCell ref="N10:N18"/>
+    <mergeCell ref="N19:N27"/>
+    <mergeCell ref="N28:N36"/>
+    <mergeCell ref="Q2:Q9"/>
+    <mergeCell ref="Q10:Q18"/>
     <mergeCell ref="Q19:Q27"/>
     <mergeCell ref="Q28:Q36"/>
     <mergeCell ref="W2:W9"/>
     <mergeCell ref="W10:W18"/>
     <mergeCell ref="W19:W27"/>
     <mergeCell ref="W28:W36"/>
-    <mergeCell ref="N2:N9"/>
-    <mergeCell ref="N10:N18"/>
-    <mergeCell ref="N19:N27"/>
-    <mergeCell ref="N28:N36"/>
     <mergeCell ref="T2:T9"/>
     <mergeCell ref="T10:T18"/>
     <mergeCell ref="T19:T27"/>
     <mergeCell ref="T28:T36"/>
-    <mergeCell ref="Q2:Q9"/>
-    <mergeCell ref="Q10:Q18"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="F10:F18"/>
-    <mergeCell ref="F19:F27"/>
-    <mergeCell ref="F28:F36"/>
-    <mergeCell ref="K2:K9"/>
-    <mergeCell ref="K10:K18"/>
-    <mergeCell ref="K19:K27"/>
-    <mergeCell ref="K28:K36"/>
+    <mergeCell ref="Z2:Z9"/>
+    <mergeCell ref="Z10:Z18"/>
+    <mergeCell ref="Z19:Z27"/>
+    <mergeCell ref="Z28:Z36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>